<commit_message>
updated docs for lcd backpack
</commit_message>
<xml_diff>
--- a/pinouts.xlsx
+++ b/pinouts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeremyNoonan\Documents\github\massey_3545_hitch_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40A61F8-E389-4773-89BC-D90844FA872E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85953BE-AE0B-496C-8E1A-4FD258B5351A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1037" yWindow="-103" windowWidth="31980" windowHeight="18720" xr2:uid="{D931354C-1D2E-4C84-8B02-94D2B887F842}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -125,24 +126,6 @@
     <t>ARD-A1</t>
   </si>
   <si>
-    <t>ARD-SCL</t>
-  </si>
-  <si>
-    <t>ARD-SDA</t>
-  </si>
-  <si>
-    <t>ARD-11</t>
-  </si>
-  <si>
-    <t>ARD-10</t>
-  </si>
-  <si>
-    <t>A-5</t>
-  </si>
-  <si>
-    <t>A-6</t>
-  </si>
-  <si>
     <t>Pull Up on Switch Board</t>
   </si>
   <si>
@@ -150,6 +133,24 @@
   </si>
   <si>
     <t>GND To SB &amp; ARD</t>
+  </si>
+  <si>
+    <t>Ard D7</t>
+  </si>
+  <si>
+    <t>Ard D6</t>
+  </si>
+  <si>
+    <t>ARD-D11</t>
+  </si>
+  <si>
+    <t>ARD-D10</t>
+  </si>
+  <si>
+    <t>ARD-A5</t>
+  </si>
+  <si>
+    <t>ARD-A4</t>
   </si>
 </sst>
 </file>
@@ -655,7 +656,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -814,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -831,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -848,10 +849,10 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.4">
@@ -868,10 +869,10 @@
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.4">
@@ -891,7 +892,7 @@
         <v>25</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.4">
@@ -962,7 +963,7 @@
         <v>26</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.4">
@@ -982,7 +983,7 @@
         <v>24</v>
       </c>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.4">
@@ -1002,7 +1003,7 @@
         <v>25</v>
       </c>
       <c r="I24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>